<commit_message>
Added tests for ACT1 maths/english, and ACT1 maths/english with no on prog in year
</commit_message>
<xml_diff>
--- a/src/PeriodEnd/PaymentsDue/SFA.DAS.ProviderPayments.Calc.PaymentsDue.UnitTests/ScenarioData/Act1MathsEnglishWIthNoOnprogInYear.xlsx
+++ b/src/PeriodEnd/PaymentsDue/SFA.DAS.ProviderPayments.Calc.PaymentsDue.UnitTests/ScenarioData/Act1MathsEnglishWIthNoOnprogInYear.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Projects\das-providerpayments\src\PeriodEnd\PaymentsDue\SFA.DAS.ProviderPayments.Calc.PaymentsDue.UnitTests\ScenarioData\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="10_ncr:8100000_{D8DF70E8-0918-4917-A736-9691FB9F372C}" xr6:coauthVersionLast="33" xr6:coauthVersionMax="33" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="10_ncr:8100000_{7C32AF66-12D9-4331-9F8D-6FBD4EBEC9A3}" xr6:coauthVersionLast="33" xr6:coauthVersionMax="33" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12223" firstSheet="1" activeTab="3" xr2:uid="{0D15C4CB-DC3A-4FDC-843E-A5A8882681B7}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12223" firstSheet="1" activeTab="6" xr2:uid="{0D15C4CB-DC3A-4FDC-843E-A5A8882681B7}"/>
   </bookViews>
   <sheets>
     <sheet name="PastPayments" sheetId="1" r:id="rId1"/>
@@ -754,8 +754,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{29113545-4422-48BA-A59E-5EDA0DBD892B}">
   <dimension ref="A1:AC12"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="C11" sqref="C11"/>
+    <sheetView topLeftCell="R1" workbookViewId="0">
+      <selection activeCell="AB5" sqref="AB5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.6" x14ac:dyDescent="0.4"/>
@@ -949,7 +949,7 @@
         <v>0</v>
       </c>
       <c r="AB2">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="AC2" t="s">
         <v>46</v>
@@ -1038,7 +1038,7 @@
         <v>0</v>
       </c>
       <c r="AB3">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="AC3" t="s">
         <v>46</v>
@@ -1127,7 +1127,7 @@
         <v>0</v>
       </c>
       <c r="AB4">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="AC4" t="s">
         <v>46</v>
@@ -1183,8 +1183,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4F20E0D4-DFE3-4584-83C1-6AB55931CA43}">
   <dimension ref="A1:AB2"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection sqref="A1:AB2"/>
+    <sheetView topLeftCell="R1" workbookViewId="0">
+      <selection activeCell="AB10" sqref="AB10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.6" x14ac:dyDescent="0.4"/>
@@ -1373,7 +1373,7 @@
         <v>0</v>
       </c>
       <c r="AB2">
-        <v>2</v>
+        <v>1</v>
       </c>
     </row>
   </sheetData>
@@ -1385,7 +1385,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{FFFDF27E-9B7C-47AE-A86A-FAE84BC024A3}">
   <dimension ref="A1:G2"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="H5" sqref="H5"/>
     </sheetView>
   </sheetViews>
@@ -1586,7 +1586,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9D57DEC8-9CE7-4F20-AF14-415D37453E52}">
   <dimension ref="A1:F2"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="E2" sqref="E2"/>
     </sheetView>
   </sheetViews>

</xml_diff>

<commit_message>
Moved datalock validation and commitment matching to a seperate service
</commit_message>
<xml_diff>
--- a/src/PeriodEnd/PaymentsDue/SFA.DAS.ProviderPayments.Calc.PaymentsDue.UnitTests/ScenarioData/Act1MathsEnglishWIthNoOnprogInYear.xlsx
+++ b/src/PeriodEnd/PaymentsDue/SFA.DAS.ProviderPayments.Calc.PaymentsDue.UnitTests/ScenarioData/Act1MathsEnglishWIthNoOnprogInYear.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Projects\das-providerpayments\src\PeriodEnd\PaymentsDue\SFA.DAS.ProviderPayments.Calc.PaymentsDue.UnitTests\ScenarioData\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Projects\SFA\DasProviderPayments\src\PeriodEnd\PaymentsDue\SFA.DAS.ProviderPayments.Calc.PaymentsDue.UnitTests\ScenarioData\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="10_ncr:8100000_{7C32AF66-12D9-4331-9F8D-6FBD4EBEC9A3}" xr6:coauthVersionLast="33" xr6:coauthVersionMax="33" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="10_ncr:8100000_{6FB695E3-54CB-45A1-9AF9-45EE8E965EF5}" xr6:coauthVersionLast="33" xr6:coauthVersionMax="33" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12223" firstSheet="1" activeTab="6" xr2:uid="{0D15C4CB-DC3A-4FDC-843E-A5A8882681B7}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12225" firstSheet="1" activeTab="5" xr2:uid="{0D15C4CB-DC3A-4FDC-843E-A5A8882681B7}"/>
   </bookViews>
   <sheets>
     <sheet name="PastPayments" sheetId="1" r:id="rId1"/>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="153" uniqueCount="58">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="156" uniqueCount="58">
   <si>
     <t>CommitmentId</t>
   </si>
@@ -565,29 +565,29 @@
       <selection activeCell="A2" sqref="A2:XFD11"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.3046875" defaultRowHeight="14.6" x14ac:dyDescent="0.4"/>
+  <sheetFormatPr defaultColWidth="9.28515625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="14.53515625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="21.69140625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="9.84375" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="16.84375" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="14.3828125" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="12.3046875" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="21.53515625" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="15.53515625" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="11.69140625" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="13.53515625" bestFit="1" customWidth="1"/>
-    <col min="11" max="12" width="15.69140625" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="13.3046875" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="21.15234375" bestFit="1" customWidth="1"/>
-    <col min="15" max="15" width="12.3828125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="14.5703125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="21.7109375" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="9.85546875" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="16.85546875" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="14.42578125" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="12.28515625" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="21.5703125" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="15.5703125" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="11.7109375" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="13.5703125" bestFit="1" customWidth="1"/>
+    <col min="11" max="12" width="15.7109375" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="13.28515625" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="21.140625" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="12.42578125" bestFit="1" customWidth="1"/>
     <col min="16" max="16" width="17" bestFit="1" customWidth="1"/>
-    <col min="17" max="17" width="26.84375" bestFit="1" customWidth="1"/>
-    <col min="18" max="18" width="25.53515625" bestFit="1" customWidth="1"/>
-    <col min="19" max="19" width="46.53515625" bestFit="1" customWidth="1"/>
+    <col min="17" max="17" width="26.85546875" bestFit="1" customWidth="1"/>
+    <col min="18" max="18" width="25.5703125" bestFit="1" customWidth="1"/>
+    <col min="19" max="19" width="46.5703125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:28" x14ac:dyDescent="0.4">
+    <row r="1" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>6</v>
       </c>
@@ -673,76 +673,76 @@
         <v>9</v>
       </c>
     </row>
-    <row r="2" spans="1:28" x14ac:dyDescent="0.4">
+    <row r="2" spans="1:28" x14ac:dyDescent="0.25">
       <c r="P2" s="1"/>
     </row>
-    <row r="3" spans="1:28" x14ac:dyDescent="0.4">
+    <row r="3" spans="1:28" x14ac:dyDescent="0.25">
       <c r="P3" s="1"/>
     </row>
-    <row r="4" spans="1:28" x14ac:dyDescent="0.4">
+    <row r="4" spans="1:28" x14ac:dyDescent="0.25">
       <c r="P4" s="1"/>
     </row>
-    <row r="5" spans="1:28" x14ac:dyDescent="0.4">
+    <row r="5" spans="1:28" x14ac:dyDescent="0.25">
       <c r="P5" s="1"/>
     </row>
-    <row r="6" spans="1:28" x14ac:dyDescent="0.4">
+    <row r="6" spans="1:28" x14ac:dyDescent="0.25">
       <c r="P6" s="1"/>
     </row>
-    <row r="7" spans="1:28" x14ac:dyDescent="0.4">
+    <row r="7" spans="1:28" x14ac:dyDescent="0.25">
       <c r="P7" s="1"/>
     </row>
-    <row r="8" spans="1:28" x14ac:dyDescent="0.4">
+    <row r="8" spans="1:28" x14ac:dyDescent="0.25">
       <c r="P8" s="1"/>
     </row>
-    <row r="9" spans="1:28" x14ac:dyDescent="0.4">
+    <row r="9" spans="1:28" x14ac:dyDescent="0.25">
       <c r="P9" s="1"/>
     </row>
-    <row r="10" spans="1:28" x14ac:dyDescent="0.4">
+    <row r="10" spans="1:28" x14ac:dyDescent="0.25">
       <c r="P10" s="1"/>
     </row>
-    <row r="11" spans="1:28" x14ac:dyDescent="0.4">
+    <row r="11" spans="1:28" x14ac:dyDescent="0.25">
       <c r="P11" s="1"/>
     </row>
-    <row r="12" spans="1:28" x14ac:dyDescent="0.4">
+    <row r="12" spans="1:28" x14ac:dyDescent="0.25">
       <c r="P12" s="1"/>
     </row>
-    <row r="13" spans="1:28" x14ac:dyDescent="0.4">
+    <row r="13" spans="1:28" x14ac:dyDescent="0.25">
       <c r="P13" s="1"/>
     </row>
-    <row r="14" spans="1:28" x14ac:dyDescent="0.4">
+    <row r="14" spans="1:28" x14ac:dyDescent="0.25">
       <c r="P14" s="1"/>
     </row>
-    <row r="15" spans="1:28" x14ac:dyDescent="0.4">
+    <row r="15" spans="1:28" x14ac:dyDescent="0.25">
       <c r="P15" s="1"/>
     </row>
-    <row r="16" spans="1:28" x14ac:dyDescent="0.4">
+    <row r="16" spans="1:28" x14ac:dyDescent="0.25">
       <c r="P16" s="1"/>
     </row>
-    <row r="17" spans="16:16" x14ac:dyDescent="0.4">
+    <row r="17" spans="16:16" x14ac:dyDescent="0.25">
       <c r="P17" s="1"/>
     </row>
-    <row r="18" spans="16:16" x14ac:dyDescent="0.4">
+    <row r="18" spans="16:16" x14ac:dyDescent="0.25">
       <c r="P18" s="1"/>
     </row>
-    <row r="19" spans="16:16" x14ac:dyDescent="0.4">
+    <row r="19" spans="16:16" x14ac:dyDescent="0.25">
       <c r="P19" s="1"/>
     </row>
-    <row r="20" spans="16:16" x14ac:dyDescent="0.4">
+    <row r="20" spans="16:16" x14ac:dyDescent="0.25">
       <c r="P20" s="1"/>
     </row>
-    <row r="21" spans="16:16" x14ac:dyDescent="0.4">
+    <row r="21" spans="16:16" x14ac:dyDescent="0.25">
       <c r="P21" s="1"/>
     </row>
-    <row r="22" spans="16:16" x14ac:dyDescent="0.4">
+    <row r="22" spans="16:16" x14ac:dyDescent="0.25">
       <c r="P22" s="1"/>
     </row>
-    <row r="23" spans="16:16" x14ac:dyDescent="0.4">
+    <row r="23" spans="16:16" x14ac:dyDescent="0.25">
       <c r="P23" s="1"/>
     </row>
-    <row r="24" spans="16:16" x14ac:dyDescent="0.4">
+    <row r="24" spans="16:16" x14ac:dyDescent="0.25">
       <c r="P24" s="1"/>
     </row>
-    <row r="25" spans="16:16" x14ac:dyDescent="0.4">
+    <row r="25" spans="16:16" x14ac:dyDescent="0.25">
       <c r="P25" s="1"/>
     </row>
   </sheetData>
@@ -758,26 +758,26 @@
       <selection activeCell="AB5" sqref="AB5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.6" x14ac:dyDescent="0.4"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="21.15234375" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="16.3828125" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="28.3046875" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="6.84375" bestFit="1" customWidth="1"/>
-    <col min="5" max="6" width="15.69140625" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="13.3046875" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="13.53515625" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="25.53515625" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="46.53515625" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="12.3828125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="21.140625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="16.42578125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="28.28515625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="6.85546875" bestFit="1" customWidth="1"/>
+    <col min="5" max="6" width="15.7109375" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="13.28515625" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="13.5703125" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="25.5703125" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="46.5703125" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="12.42578125" bestFit="1" customWidth="1"/>
     <col min="12" max="12" width="17" bestFit="1" customWidth="1"/>
-    <col min="13" max="20" width="17.69140625" bestFit="1" customWidth="1"/>
-    <col min="21" max="21" width="17.69140625" style="3" bestFit="1" customWidth="1"/>
-    <col min="22" max="27" width="17.69140625" bestFit="1" customWidth="1"/>
-    <col min="28" max="28" width="26.84375" bestFit="1" customWidth="1"/>
+    <col min="13" max="20" width="17.7109375" bestFit="1" customWidth="1"/>
+    <col min="21" max="21" width="17.7109375" style="3" bestFit="1" customWidth="1"/>
+    <col min="22" max="27" width="17.7109375" bestFit="1" customWidth="1"/>
+    <col min="28" max="28" width="26.85546875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:29" x14ac:dyDescent="0.4">
+    <row r="1" spans="1:29" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>6</v>
       </c>
@@ -866,7 +866,7 @@
         <v>45</v>
       </c>
     </row>
-    <row r="2" spans="1:29" x14ac:dyDescent="0.4">
+    <row r="2" spans="1:29" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>55</v>
       </c>
@@ -955,7 +955,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="3" spans="1:29" x14ac:dyDescent="0.4">
+    <row r="3" spans="1:29" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>50</v>
       </c>
@@ -1044,7 +1044,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="4" spans="1:29" x14ac:dyDescent="0.4">
+    <row r="4" spans="1:29" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>52</v>
       </c>
@@ -1133,42 +1133,42 @@
         <v>46</v>
       </c>
     </row>
-    <row r="5" spans="1:29" x14ac:dyDescent="0.4">
+    <row r="5" spans="1:29" x14ac:dyDescent="0.25">
       <c r="B5" s="2"/>
       <c r="C5" s="2"/>
       <c r="L5" s="2"/>
     </row>
-    <row r="6" spans="1:29" x14ac:dyDescent="0.4">
+    <row r="6" spans="1:29" x14ac:dyDescent="0.25">
       <c r="B6" s="2"/>
       <c r="C6" s="2"/>
       <c r="L6" s="2"/>
     </row>
-    <row r="7" spans="1:29" x14ac:dyDescent="0.4">
+    <row r="7" spans="1:29" x14ac:dyDescent="0.25">
       <c r="B7" s="2"/>
       <c r="C7" s="2"/>
       <c r="L7" s="2"/>
     </row>
-    <row r="8" spans="1:29" x14ac:dyDescent="0.4">
+    <row r="8" spans="1:29" x14ac:dyDescent="0.25">
       <c r="B8" s="2"/>
       <c r="C8" s="2"/>
       <c r="L8" s="2"/>
     </row>
-    <row r="9" spans="1:29" x14ac:dyDescent="0.4">
+    <row r="9" spans="1:29" x14ac:dyDescent="0.25">
       <c r="B9" s="2"/>
       <c r="C9" s="2"/>
       <c r="L9" s="2"/>
     </row>
-    <row r="10" spans="1:29" x14ac:dyDescent="0.4">
+    <row r="10" spans="1:29" x14ac:dyDescent="0.25">
       <c r="B10" s="2"/>
       <c r="C10" s="2"/>
       <c r="L10" s="2"/>
     </row>
-    <row r="11" spans="1:29" x14ac:dyDescent="0.4">
+    <row r="11" spans="1:29" x14ac:dyDescent="0.25">
       <c r="B11" s="2"/>
       <c r="C11" s="2"/>
       <c r="L11" s="2"/>
     </row>
-    <row r="12" spans="1:29" x14ac:dyDescent="0.4">
+    <row r="12" spans="1:29" x14ac:dyDescent="0.25">
       <c r="B12" s="2"/>
       <c r="C12" s="2"/>
       <c r="L12" s="2"/>
@@ -1187,24 +1187,24 @@
       <selection activeCell="AB10" sqref="AB10"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.6" x14ac:dyDescent="0.4"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="21.15234375" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="16.3828125" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="28.3046875" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="6.84375" bestFit="1" customWidth="1"/>
-    <col min="5" max="6" width="15.69140625" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="13.3046875" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="13.53515625" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="25.53515625" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="46.53515625" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="12.3828125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="21.140625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="16.42578125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="28.28515625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="6.85546875" bestFit="1" customWidth="1"/>
+    <col min="5" max="6" width="15.7109375" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="13.28515625" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="13.5703125" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="25.5703125" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="46.5703125" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="12.42578125" bestFit="1" customWidth="1"/>
     <col min="12" max="12" width="17" bestFit="1" customWidth="1"/>
-    <col min="13" max="27" width="17.69140625" bestFit="1" customWidth="1"/>
-    <col min="28" max="28" width="26.84375" bestFit="1" customWidth="1"/>
+    <col min="13" max="27" width="17.7109375" bestFit="1" customWidth="1"/>
+    <col min="28" max="28" width="26.85546875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:28" x14ac:dyDescent="0.4">
+    <row r="1" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>6</v>
       </c>
@@ -1290,7 +1290,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="2" spans="1:28" x14ac:dyDescent="0.4">
+    <row r="2" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>12</v>
       </c>
@@ -1389,16 +1389,16 @@
       <selection activeCell="H5" sqref="H5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.6" x14ac:dyDescent="0.4"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="21.15234375" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="14.53515625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="11.69140625" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="6.84375" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="21.140625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="14.5703125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="11.7109375" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="6.85546875" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="8" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.4">
+    <row r="1" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>6</v>
       </c>
@@ -1418,7 +1418,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.4">
+    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>50</v>
       </c>
@@ -1454,9 +1454,9 @@
       <selection activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.6" x14ac:dyDescent="0.4"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.4">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>6</v>
       </c>
@@ -1473,29 +1473,29 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{DCAC57EC-71F8-44A3-A54A-6DD5C7C43883}">
   <dimension ref="A1:P7"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A2" sqref="A2:XFD3"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A2" sqref="A2:P2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.6" x14ac:dyDescent="0.4"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="14.53515625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="11.69140625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="9.84375" bestFit="1" customWidth="1"/>
-    <col min="4" max="5" width="10.69140625" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="11.3046875" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="13.53515625" bestFit="1" customWidth="1"/>
-    <col min="8" max="9" width="15.69140625" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="13.3046875" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="14.3828125" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="7.53515625" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="13.53515625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="14.5703125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="11.7109375" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="9.85546875" bestFit="1" customWidth="1"/>
+    <col min="4" max="5" width="10.7109375" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="11.28515625" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="13.5703125" bestFit="1" customWidth="1"/>
+    <col min="8" max="9" width="15.7109375" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="13.28515625" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="14.42578125" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="7.5703125" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="13.5703125" bestFit="1" customWidth="1"/>
     <col min="14" max="14" width="11" bestFit="1" customWidth="1"/>
-    <col min="15" max="15" width="33.3828125" bestFit="1" customWidth="1"/>
-    <col min="16" max="16" width="20.69140625" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="33.42578125" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="20.7109375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:16" x14ac:dyDescent="0.4">
+    <row r="1" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -1545,34 +1545,78 @@
         <v>42</v>
       </c>
     </row>
-    <row r="2" spans="1:16" x14ac:dyDescent="0.4">
-      <c r="D2" s="2"/>
-      <c r="E2" s="2"/>
-      <c r="M2" s="2"/>
-      <c r="N2" s="2"/>
-    </row>
-    <row r="3" spans="1:16" x14ac:dyDescent="0.4">
+    <row r="2" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A2">
+        <v>1</v>
+      </c>
+      <c r="B2" t="s">
+        <v>57</v>
+      </c>
+      <c r="C2">
+        <v>0</v>
+      </c>
+      <c r="D2" s="2">
+        <v>42948</v>
+      </c>
+      <c r="E2" s="2">
+        <v>43313</v>
+      </c>
+      <c r="F2">
+        <v>15000</v>
+      </c>
+      <c r="G2">
+        <v>23</v>
+      </c>
+      <c r="H2">
+        <v>2</v>
+      </c>
+      <c r="I2">
+        <v>403</v>
+      </c>
+      <c r="J2">
+        <v>1</v>
+      </c>
+      <c r="K2">
+        <v>1</v>
+      </c>
+      <c r="L2">
+        <v>1</v>
+      </c>
+      <c r="M2" s="2">
+        <v>42948</v>
+      </c>
+      <c r="N2" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="O2" t="s">
+        <v>12</v>
+      </c>
+      <c r="P2" s="1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="3" spans="1:16" x14ac:dyDescent="0.25">
       <c r="D3" s="2"/>
       <c r="E3" s="2"/>
       <c r="M3" s="2"/>
     </row>
-    <row r="4" spans="1:16" x14ac:dyDescent="0.4">
+    <row r="4" spans="1:16" x14ac:dyDescent="0.25">
       <c r="D4" s="2"/>
       <c r="E4" s="2"/>
       <c r="M4" s="2"/>
       <c r="N4" s="2"/>
     </row>
-    <row r="5" spans="1:16" x14ac:dyDescent="0.4">
+    <row r="5" spans="1:16" x14ac:dyDescent="0.25">
       <c r="D5" s="2"/>
       <c r="E5" s="2"/>
       <c r="M5" s="2"/>
     </row>
-    <row r="6" spans="1:16" x14ac:dyDescent="0.4">
+    <row r="6" spans="1:16" x14ac:dyDescent="0.25">
       <c r="D6" s="2"/>
       <c r="E6" s="2"/>
       <c r="M6" s="2"/>
     </row>
-    <row r="7" spans="1:16" x14ac:dyDescent="0.4">
+    <row r="7" spans="1:16" x14ac:dyDescent="0.25">
       <c r="D7" s="2"/>
       <c r="E7" s="2"/>
       <c r="M7" s="2"/>
@@ -1586,19 +1630,19 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9D57DEC8-9CE7-4F20-AF14-415D37453E52}">
   <dimension ref="A1:F2"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="E2" sqref="E2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.6" x14ac:dyDescent="0.4"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="2" width="17.07421875" customWidth="1"/>
-    <col min="3" max="3" width="11.53515625" customWidth="1"/>
-    <col min="4" max="4" width="20.53515625" customWidth="1"/>
-    <col min="5" max="5" width="21.765625" customWidth="1"/>
+    <col min="1" max="2" width="17.140625" customWidth="1"/>
+    <col min="3" max="3" width="11.5703125" customWidth="1"/>
+    <col min="4" max="4" width="20.5703125" customWidth="1"/>
+    <col min="5" max="5" width="21.7109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.4">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>53</v>
       </c>
@@ -1615,7 +1659,7 @@
         <v>49</v>
       </c>
     </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.4">
+    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A2">
         <v>2017</v>
       </c>

</xml_diff>